<commit_message>
Add f1040s3-2021.xlsx to index page
</commit_message>
<xml_diff>
--- a/Federal/f1040s3-2021.xlsx
+++ b/Federal/f1040s3-2021.xlsx
@@ -665,15 +665,15 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.63671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.88"/>
   </cols>
   <sheetData>
@@ -695,7 +695,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>